<commit_message>
completed tabs for the rest of the code tables
</commit_message>
<xml_diff>
--- a/r-load/NIBRSCodeTables.xlsx
+++ b/r-load/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30920" yWindow="-140" windowWidth="25600" windowHeight="14320" tabRatio="500" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="29500" yWindow="-80" windowWidth="25600" windowHeight="14320" tabRatio="705"/>
   </bookViews>
   <sheets>
     <sheet name="SegmentActionTypeType" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,25 @@
     <sheet name="TypeOfCriminalActivityType" sheetId="7" r:id="rId7"/>
     <sheet name="TypeOfWeaponForceInvolvedType" sheetId="8" r:id="rId8"/>
     <sheet name="BiasMotivationType" sheetId="9" r:id="rId9"/>
+    <sheet name="TypePropertyLossEtcType" sheetId="10" r:id="rId10"/>
+    <sheet name="PropertyDescriptionType" sheetId="11" r:id="rId11"/>
+    <sheet name="SuspectedDrugTypeType" sheetId="12" r:id="rId12"/>
+    <sheet name="TypeDrugMeasurementType" sheetId="13" r:id="rId13"/>
+    <sheet name="TypeOfVictimType" sheetId="14" r:id="rId14"/>
+    <sheet name="TypeOfOfficerActivityCircumstan" sheetId="15" r:id="rId15"/>
+    <sheet name="OfficerAssignmentTypeType" sheetId="16" r:id="rId16"/>
+    <sheet name="SexOfPersonType" sheetId="17" r:id="rId17"/>
+    <sheet name="RaceOfPersonType" sheetId="18" r:id="rId18"/>
+    <sheet name="EthnicityOfPersonType" sheetId="19" r:id="rId19"/>
+    <sheet name="ResidentStatusOfPersonType" sheetId="20" r:id="rId20"/>
+    <sheet name="AggravatedAssaultHomicideCircum" sheetId="21" r:id="rId21"/>
+    <sheet name="AdditionalJustifiableHomicideCi" sheetId="22" r:id="rId22"/>
+    <sheet name="TypeInjuryType" sheetId="23" r:id="rId23"/>
+    <sheet name="RelationshipsVictimToOffendersT" sheetId="24" r:id="rId24"/>
+    <sheet name="TypeOfArrestType" sheetId="25" r:id="rId25"/>
+    <sheet name="MultipleArresteeSegmentsIndicat" sheetId="26" r:id="rId26"/>
+    <sheet name="ArresteeWasArmedWithType" sheetId="27" r:id="rId27"/>
+    <sheet name="DispositionOfArresteeUnder18Typ" sheetId="28" r:id="rId28"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="575">
   <si>
     <t>I</t>
   </si>
@@ -876,13 +895,889 @@
   </si>
   <si>
     <t>Anti-Transgender</t>
+  </si>
+  <si>
+    <t>Burned (includes damage caused in fighting the fire)</t>
+  </si>
+  <si>
+    <t>Counterfeited/Forged</t>
+  </si>
+  <si>
+    <t>Destroyed/Damaged/Vandalized</t>
+  </si>
+  <si>
+    <t>Recovered (to impound property that was previously stolen)</t>
+  </si>
+  <si>
+    <t>Seized (to impound property that was not previously stolen)</t>
+  </si>
+  <si>
+    <t>Stolen/Etc. (includes bribed, defrauded, embezzled, extorted, ransomed, robbed, etc.)</t>
+  </si>
+  <si>
+    <t>Aircraft</t>
+  </si>
+  <si>
+    <t>Automobiles</t>
+  </si>
+  <si>
+    <t>Bicycles</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>buses</t>
+  </si>
+  <si>
+    <t>clothes/ furs</t>
+  </si>
+  <si>
+    <t>computer hard/ software</t>
+  </si>
+  <si>
+    <t>consumable goods</t>
+  </si>
+  <si>
+    <t>credit/ debit cards</t>
+  </si>
+  <si>
+    <t>drugs/ narcotics</t>
+  </si>
+  <si>
+    <t>drug equipment</t>
+  </si>
+  <si>
+    <t>farm equipment</t>
+  </si>
+  <si>
+    <t>firearms</t>
+  </si>
+  <si>
+    <t>gambling equipment</t>
+  </si>
+  <si>
+    <t>industrial equipment</t>
+  </si>
+  <si>
+    <t>household goods</t>
+  </si>
+  <si>
+    <t>jewelry/ precious metals</t>
+  </si>
+  <si>
+    <t>livestock</t>
+  </si>
+  <si>
+    <t>merchandise</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>negotiable instruments</t>
+  </si>
+  <si>
+    <t>non negotiable instruments</t>
+  </si>
+  <si>
+    <t>office equipment</t>
+  </si>
+  <si>
+    <t>other motor vehicles</t>
+  </si>
+  <si>
+    <t>purse/ wallet</t>
+  </si>
+  <si>
+    <t>radio/ tv/ vcr</t>
+  </si>
+  <si>
+    <t>recordings</t>
+  </si>
+  <si>
+    <t>recreational vehicles</t>
+  </si>
+  <si>
+    <t>structure/ single dwelling</t>
+  </si>
+  <si>
+    <t>structure/ other residence</t>
+  </si>
+  <si>
+    <t>structure/ other commercial</t>
+  </si>
+  <si>
+    <t>structure/ other industrial</t>
+  </si>
+  <si>
+    <t>structure/ public</t>
+  </si>
+  <si>
+    <t>structure/ storage</t>
+  </si>
+  <si>
+    <t>structure/ other</t>
+  </si>
+  <si>
+    <t>tools</t>
+  </si>
+  <si>
+    <t>trucks</t>
+  </si>
+  <si>
+    <t>vehicle parts</t>
+  </si>
+  <si>
+    <t>watercraft</t>
+  </si>
+  <si>
+    <t>Aircraft Parts/ Accessories</t>
+  </si>
+  <si>
+    <t>Artistic Supplies/ Accessories</t>
+  </si>
+  <si>
+    <t>Building Materials</t>
+  </si>
+  <si>
+    <t>Camping/ Hunting/ Fishing Equipment/ Supplies</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Collections/ Collectibles</t>
+  </si>
+  <si>
+    <t>Crops</t>
+  </si>
+  <si>
+    <t>Documents/ Personal or Business</t>
+  </si>
+  <si>
+    <t>Firearm Accessories</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Identity Documents</t>
+  </si>
+  <si>
+    <t>Identity-Intangible</t>
+  </si>
+  <si>
+    <t>Law Enforcement Equipment</t>
+  </si>
+  <si>
+    <t>Lawn/ Yard/ Garden Equipment</t>
+  </si>
+  <si>
+    <t>Logging Equipment</t>
+  </si>
+  <si>
+    <t>Medical/ Medical Lab Equipment</t>
+  </si>
+  <si>
+    <t>Metals, Non-Precious</t>
+  </si>
+  <si>
+    <t>Musical Instruments</t>
+  </si>
+  <si>
+    <t>Pets</t>
+  </si>
+  <si>
+    <t>Photographic/ Optical Equipment</t>
+  </si>
+  <si>
+    <t>Portable Electronic Communications</t>
+  </si>
+  <si>
+    <t>Recreational/ Sports Equipment</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Trailers</t>
+  </si>
+  <si>
+    <t>Watercraft Equipment/ Parts/ Accessories</t>
+  </si>
+  <si>
+    <t>Weapons-Other</t>
+  </si>
+  <si>
+    <t>pending inventory</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>crack cocaine</t>
+  </si>
+  <si>
+    <t>cocaine</t>
+  </si>
+  <si>
+    <t>hashish</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
+    <t>marijuana</t>
+  </si>
+  <si>
+    <t>morphine</t>
+  </si>
+  <si>
+    <t>opium</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>other narcotics</t>
+  </si>
+  <si>
+    <t>LSD</t>
+  </si>
+  <si>
+    <t>PCP</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>other hallucinogens</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>meth/amphetamines</t>
+  </si>
+  <si>
+    <t>other stimulants</t>
+  </si>
+  <si>
+    <t>barbiturates</t>
+  </si>
+  <si>
+    <t>other depressants</t>
+  </si>
+  <si>
+    <t>other drugs</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>more than 3 types</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>Dosage Units/Items</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>Fluid Ounce</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>Gallon</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>Gram</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>Kilogram</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>Liter</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Milliliter</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>Number of Plants</t>
+  </si>
+  <si>
+    <t>OZ</t>
+  </si>
+  <si>
+    <t>Ounce</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>Not Reported</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Financial Institution</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Religious Organization</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Society/Public</t>
+  </si>
+  <si>
+    <t>Law Enforcement Officer (valid for offenses 09A, 13A, 13B, and 13C only)</t>
+  </si>
+  <si>
+    <t>Responding to Disturbance Call (Family Quarrels, Person with Firearm, Etc.)</t>
+  </si>
+  <si>
+    <t>Burglaries in Progress or Pursuing Burglary Suspects</t>
+  </si>
+  <si>
+    <t>Robberies in Progress or Pursuing Robbery Suspects</t>
+  </si>
+  <si>
+    <t>Attempting Other Arrests</t>
+  </si>
+  <si>
+    <t>Civil Disorder (Riot, Mass Disobedience)</t>
+  </si>
+  <si>
+    <t>Handling, Transporting, Custody of Prisoners</t>
+  </si>
+  <si>
+    <t>Investigating Suspicious Persons or Circumstances</t>
+  </si>
+  <si>
+    <t>Ambush - No Warning</t>
+  </si>
+  <si>
+    <t>Mentally Deranged Assailant</t>
+  </si>
+  <si>
+    <t>Traffic Pursuits and Stops</t>
+  </si>
+  <si>
+    <t>All Other</t>
+  </si>
+  <si>
+    <t>Two-Officer Vehicle - pertains to uniformed officers</t>
+  </si>
+  <si>
+    <t>One-Officer Vehicle (Alone) - pertains to uniformed officers</t>
+  </si>
+  <si>
+    <t>One-Officer Vehicle (Assisted) - pertains to uniformed officers</t>
+  </si>
+  <si>
+    <t>Detective or Special Assignment (Alone) - pertains to nonuniformed officers</t>
+  </si>
+  <si>
+    <t>Detective or Special Assignment (Assisted) - pertains to nonuniformed officers</t>
+  </si>
+  <si>
+    <t>Other (Alone) - pertains to officers in other capacities, such as foot patrol, off duty, etc.</t>
+  </si>
+  <si>
+    <t>Other (Assisted) - pertains to officers in other capacities, such as foot patrol, off duty, etc.</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>UNKNOWN - FOR UNIDENTIFIED ONLY</t>
+  </si>
+  <si>
+    <t>ASIAN:  A person having origins in any of the original peoples of the Far East, Southeast Asia, or the Indian subcontinent including, for example, Cambodia, China, India, Japan, Korea, Malaysia, Pakistan, the Philippine Islands, Thailand, and Vietnam.</t>
+  </si>
+  <si>
+    <t>BLACK or AFRICAN AMERICAN:  A person having origins in any of the black racial groups of Africa.</t>
+  </si>
+  <si>
+    <t>AMERICAN INDIAN or ALASKA NATIVE:  A person having origins in any of the original peoples of the Americas and maintaining cultural identification through tribal affiliations or community recognition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNKNOWN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHITE:  A person having origins in any of the original peoples of Europe, North Africa, or Middle East.  </t>
+  </si>
+  <si>
+    <t>NATIVE HAWAIIAN or OTHER PACIFIC ISLANDER:  A person having origins in any of the original peoples of Hawaii, Guam, Samoa, or other Pacific Islands.  The term "Native Hawaiian" does not include individuals who are native to the State of Hawaii by virtue of being born there.  However, the following Pacific Islander groups are included:  Carolinian, Fijian, Kosraean, Melanesian, Micronesian, Northern Mariana Islander, Palauan, Papua New Guinean, Ponapean (Pohnpelan), Polynesian, Solomon Islander, Tahitian, Tarawa Islander, Tokelauan, Tongan, Trukese (Chuukese), and Yapese.</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>non Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Nonresident</t>
+  </si>
+  <si>
+    <t>Resident</t>
+  </si>
+  <si>
+    <t>Argument</t>
+  </si>
+  <si>
+    <t>Assault on Law Enforcement Officer(s)</t>
+  </si>
+  <si>
+    <t>Drug Dealing</t>
+  </si>
+  <si>
+    <t>Gangland (Organized Crime Involvement)</t>
+  </si>
+  <si>
+    <t>Juvenile Gang</t>
+  </si>
+  <si>
+    <t>Lovers Quarrel</t>
+  </si>
+  <si>
+    <t>Mercy Killing (Not applicable to Aggravated Assault)</t>
+  </si>
+  <si>
+    <t>Other Felony Involved</t>
+  </si>
+  <si>
+    <t>Other Circumstances</t>
+  </si>
+  <si>
+    <t>Unknown Circumstances</t>
+  </si>
+  <si>
+    <t>Child Playing With Weapon</t>
+  </si>
+  <si>
+    <t>Gun-Cleaning Accident</t>
+  </si>
+  <si>
+    <t>Hunting Accident</t>
+  </si>
+  <si>
+    <t>Other Negligent Weapon Handling</t>
+  </si>
+  <si>
+    <t>Other Negligent Killings</t>
+  </si>
+  <si>
+    <t>Criminal Killed by Private Citizen</t>
+  </si>
+  <si>
+    <t>Criminal Killed by Police Officer</t>
+  </si>
+  <si>
+    <t>Criminal Attacked Police Officer and That Officer Killed Criminal</t>
+  </si>
+  <si>
+    <t>Criminal Attacked Police Officer and Criminal Killed by Another Police Officer</t>
+  </si>
+  <si>
+    <t>Criminal Attacked a Civilian</t>
+  </si>
+  <si>
+    <t>Criminal Attempted Flight From a Crime</t>
+  </si>
+  <si>
+    <t>Criminal Killed in Commission of a Crime</t>
+  </si>
+  <si>
+    <t>Criminal Resisted Arrest</t>
+  </si>
+  <si>
+    <t>Unable to Determine/Not Enough Information</t>
+  </si>
+  <si>
+    <t>apparent broken bones</t>
+  </si>
+  <si>
+    <t>possible internal injury</t>
+  </si>
+  <si>
+    <t>severe laceration</t>
+  </si>
+  <si>
+    <t>minor injury</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>other major injury</t>
+  </si>
+  <si>
+    <t>loss of teeth</t>
+  </si>
+  <si>
+    <t>unconscious</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>Victim Was Acquaintance</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Victim Was Babysittee (the baby)</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>Victim Was Boyfriend/Girlfriend</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>Victim Was Child of Boyfriend or Girlfriend</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>Victim Was Child</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Victim Was Common-Law Spouse</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Victim was Employee</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>Victim was Employer</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Victim Was Friend</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>Victim Was Grandchild</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>Victim Was Grandparent</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Homosexual Relationship</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Victim Was In-law</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Victim Was Neighbor</t>
+  </si>
+  <si>
+    <t>OF</t>
+  </si>
+  <si>
+    <t>Victim Was Other Family Member</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Victim was Otherwise Known</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Victim Was Parent</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>Relationship Unknown</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>Victim Was Sibling (brother or sister)</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Victim Was Stepchild</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Victim Was Spouse</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Victim Was Stepparent</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Victim Was Stepsibling (stepbrother or stepsister)</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Victim Was Stranger</t>
+  </si>
+  <si>
+    <t>VO</t>
+  </si>
+  <si>
+    <t>Victim Was Offender</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>Victim was Ex-Spouse</t>
+  </si>
+  <si>
+    <t>on view</t>
+  </si>
+  <si>
+    <t>summoned/cited</t>
+  </si>
+  <si>
+    <t>taken into custody</t>
+  </si>
+  <si>
+    <t>Count Arrestee</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Unarmed</t>
+  </si>
+  <si>
+    <t>Firearm (type not stated)</t>
+  </si>
+  <si>
+    <t>Lethal Cutting Instrument (e.g., switchblade knife or martial arts stars)</t>
+  </si>
+  <si>
+    <t>Club/Blackjack/Brass Knuckles</t>
+  </si>
+  <si>
+    <t>Firearm (type not stated) - Automatic</t>
+  </si>
+  <si>
+    <t>12A</t>
+  </si>
+  <si>
+    <t>Handgun - Automatic</t>
+  </si>
+  <si>
+    <t>Rifle - Automatic</t>
+  </si>
+  <si>
+    <t>14A</t>
+  </si>
+  <si>
+    <t>Shotgun - Automatic</t>
+  </si>
+  <si>
+    <t>15A</t>
+  </si>
+  <si>
+    <t>Other Firearm - Automatic</t>
+  </si>
+  <si>
+    <t>Handled Within Department</t>
+  </si>
+  <si>
+    <t>Referred to Other Authorities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -913,6 +1808,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -931,7 +1831,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -961,6 +1861,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -969,7 +1914,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="74">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -984,6 +1929,28 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -998,7 +1965,30 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="73"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1329,7 +2319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1404,6 +2394,1950 @@
       </c>
       <c r="C6" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C28" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C30" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C31" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C32" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C33" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C34" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C35" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C36" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C43" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C50" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C51" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C52" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C53" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C54" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C55" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C56" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C57" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C58" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C59" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C60" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C61" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C62" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C63" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C64" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C65" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C66" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C67" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C68" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C69" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>394</v>
+      </c>
+      <c r="C9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>400</v>
+      </c>
+      <c r="C13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C16" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>406</v>
+      </c>
+      <c r="C18" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>409</v>
+      </c>
+      <c r="C20" t="s">
+        <v>410</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C9" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>427</v>
+      </c>
+      <c r="C10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>429</v>
+      </c>
+      <c r="C11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>431</v>
+      </c>
+      <c r="C12" t="s">
+        <v>432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="60.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>438</v>
+      </c>
+      <c r="C9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="62.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>400</v>
+      </c>
+      <c r="C8" t="s">
+        <v>458</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="255.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -1502,6 +4436,1202 @@
       </c>
       <c r="C7" t="s">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" t="s">
+        <v>495</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>400</v>
+      </c>
+      <c r="C4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" t="s">
+        <v>503</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C3" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>508</v>
+      </c>
+      <c r="C4" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C5" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>512</v>
+      </c>
+      <c r="C6" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>514</v>
+      </c>
+      <c r="C7" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>516</v>
+      </c>
+      <c r="C8" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>518</v>
+      </c>
+      <c r="C9" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>520</v>
+      </c>
+      <c r="C10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>522</v>
+      </c>
+      <c r="C11" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>524</v>
+      </c>
+      <c r="C12" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>526</v>
+      </c>
+      <c r="C13" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>528</v>
+      </c>
+      <c r="C14" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>530</v>
+      </c>
+      <c r="C15" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>532</v>
+      </c>
+      <c r="C16" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>534</v>
+      </c>
+      <c r="C17" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>536</v>
+      </c>
+      <c r="C18" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C19" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>540</v>
+      </c>
+      <c r="C20" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>542</v>
+      </c>
+      <c r="C21" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>544</v>
+      </c>
+      <c r="C22" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>546</v>
+      </c>
+      <c r="C23" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>548</v>
+      </c>
+      <c r="C24" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>550</v>
+      </c>
+      <c r="C25" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>552</v>
+      </c>
+      <c r="C26" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>554</v>
+      </c>
+      <c r="C27" t="s">
+        <v>555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>566</v>
+      </c>
+      <c r="C11" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>569</v>
+      </c>
+      <c r="C13" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>571</v>
+      </c>
+      <c r="C14" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C3" t="s">
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -2257,7 +6387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
@@ -3222,8 +7352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3553,6 +7683,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added TOC tab to spreadsheet
</commit_message>
<xml_diff>
--- a/r-load/NIBRSCodeTables.xlsx
+++ b/r-load/NIBRSCodeTables.xlsx
@@ -4,37 +4,38 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29500" yWindow="-80" windowWidth="25600" windowHeight="14320" tabRatio="705"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="705"/>
   </bookViews>
   <sheets>
-    <sheet name="SegmentActionTypeType" sheetId="1" r:id="rId1"/>
-    <sheet name="ClearedExceptionallyType" sheetId="2" r:id="rId2"/>
-    <sheet name="UCROffenseCodeType" sheetId="3" r:id="rId3"/>
-    <sheet name="OffenderSuspectedOfUsingType" sheetId="4" r:id="rId4"/>
-    <sheet name="LocationTypeType" sheetId="5" r:id="rId5"/>
-    <sheet name="MethodOfEntryType" sheetId="6" r:id="rId6"/>
-    <sheet name="TypeOfCriminalActivityType" sheetId="7" r:id="rId7"/>
-    <sheet name="TypeOfWeaponForceInvolvedType" sheetId="8" r:id="rId8"/>
-    <sheet name="BiasMotivationType" sheetId="9" r:id="rId9"/>
-    <sheet name="TypePropertyLossEtcType" sheetId="10" r:id="rId10"/>
-    <sheet name="PropertyDescriptionType" sheetId="11" r:id="rId11"/>
-    <sheet name="SuspectedDrugTypeType" sheetId="12" r:id="rId12"/>
-    <sheet name="TypeDrugMeasurementType" sheetId="13" r:id="rId13"/>
-    <sheet name="TypeOfVictimType" sheetId="14" r:id="rId14"/>
-    <sheet name="TypeOfOfficerActivityCircumstan" sheetId="15" r:id="rId15"/>
-    <sheet name="OfficerAssignmentTypeType" sheetId="16" r:id="rId16"/>
-    <sheet name="SexOfPersonType" sheetId="17" r:id="rId17"/>
-    <sheet name="RaceOfPersonType" sheetId="18" r:id="rId18"/>
-    <sheet name="EthnicityOfPersonType" sheetId="19" r:id="rId19"/>
-    <sheet name="ResidentStatusOfPersonType" sheetId="20" r:id="rId20"/>
-    <sheet name="AggravatedAssaultHomicideCircum" sheetId="21" r:id="rId21"/>
-    <sheet name="AdditionalJustifiableHomicideCi" sheetId="22" r:id="rId22"/>
-    <sheet name="TypeInjuryType" sheetId="23" r:id="rId23"/>
-    <sheet name="RelationshipsVictimToOffendersT" sheetId="24" r:id="rId24"/>
-    <sheet name="TypeOfArrestType" sheetId="25" r:id="rId25"/>
-    <sheet name="MultipleArresteeSegmentsIndicat" sheetId="26" r:id="rId26"/>
-    <sheet name="ArresteeWasArmedWithType" sheetId="27" r:id="rId27"/>
-    <sheet name="DispositionOfArresteeUnder18Typ" sheetId="28" r:id="rId28"/>
+    <sheet name="TOC" sheetId="29" r:id="rId1"/>
+    <sheet name="SegmentActionTypeType" sheetId="1" r:id="rId2"/>
+    <sheet name="ClearedExceptionallyType" sheetId="2" r:id="rId3"/>
+    <sheet name="UCROffenseCodeType" sheetId="3" r:id="rId4"/>
+    <sheet name="OffenderSuspectedOfUsingType" sheetId="4" r:id="rId5"/>
+    <sheet name="LocationTypeType" sheetId="5" r:id="rId6"/>
+    <sheet name="MethodOfEntryType" sheetId="6" r:id="rId7"/>
+    <sheet name="TypeOfCriminalActivityType" sheetId="7" r:id="rId8"/>
+    <sheet name="TypeOfWeaponForceInvolvedType" sheetId="8" r:id="rId9"/>
+    <sheet name="BiasMotivationType" sheetId="9" r:id="rId10"/>
+    <sheet name="TypePropertyLossEtcType" sheetId="10" r:id="rId11"/>
+    <sheet name="PropertyDescriptionType" sheetId="11" r:id="rId12"/>
+    <sheet name="SuspectedDrugTypeType" sheetId="12" r:id="rId13"/>
+    <sheet name="TypeDrugMeasurementType" sheetId="13" r:id="rId14"/>
+    <sheet name="TypeOfVictimType" sheetId="14" r:id="rId15"/>
+    <sheet name="OfficerActivityCircumstanceType" sheetId="15" r:id="rId16"/>
+    <sheet name="OfficerAssignmentTypeType" sheetId="16" r:id="rId17"/>
+    <sheet name="SexOfPersonType" sheetId="17" r:id="rId18"/>
+    <sheet name="RaceOfPersonType" sheetId="18" r:id="rId19"/>
+    <sheet name="EthnicityOfPersonType" sheetId="19" r:id="rId20"/>
+    <sheet name="ResidentStatusOfPersonType" sheetId="20" r:id="rId21"/>
+    <sheet name="AggravatedAssaultHomicideCircum" sheetId="21" r:id="rId22"/>
+    <sheet name="AdditionalJustifiableHomicideCi" sheetId="22" r:id="rId23"/>
+    <sheet name="TypeInjuryType" sheetId="23" r:id="rId24"/>
+    <sheet name="RelationshipsVictimToOffendersT" sheetId="24" r:id="rId25"/>
+    <sheet name="TypeOfArrestType" sheetId="25" r:id="rId26"/>
+    <sheet name="MultipleArresteeSegmentsIndicat" sheetId="26" r:id="rId27"/>
+    <sheet name="ArresteeWasArmedWithType" sheetId="27" r:id="rId28"/>
+    <sheet name="DispositionOfArresteeUnder18Typ" sheetId="28" r:id="rId29"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="610">
   <si>
     <t>I</t>
   </si>
@@ -1771,6 +1772,111 @@
   </si>
   <si>
     <t>Referred to Other Authorities</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>SegmentActionTypeType</t>
+  </si>
+  <si>
+    <t>ClearedExceptionallyType</t>
+  </si>
+  <si>
+    <t>UCROffenseCodeType</t>
+  </si>
+  <si>
+    <t>OffenderSuspectedOfUsingType</t>
+  </si>
+  <si>
+    <t>LocationTypeType</t>
+  </si>
+  <si>
+    <t>MethodOfEntryType</t>
+  </si>
+  <si>
+    <t>TypeOfCriminalActivityType</t>
+  </si>
+  <si>
+    <t>TypeOfWeaponForceInvolvedType</t>
+  </si>
+  <si>
+    <t>BiasMotivationType</t>
+  </si>
+  <si>
+    <t>TypePropertyLossEctType</t>
+  </si>
+  <si>
+    <t>PropertyDescriptionType</t>
+  </si>
+  <si>
+    <t>SuspectedDrugTypeType</t>
+  </si>
+  <si>
+    <t>TypeDrugMeasurementType</t>
+  </si>
+  <si>
+    <t>TypeOfVictimType</t>
+  </si>
+  <si>
+    <t>OfficerActivityCircumstanceType</t>
+  </si>
+  <si>
+    <t>OfficerAssignmentTypeType</t>
+  </si>
+  <si>
+    <t>SexOfPersonType</t>
+  </si>
+  <si>
+    <t>RaceOfPersonType</t>
+  </si>
+  <si>
+    <t>EthnicityOfPersonType</t>
+  </si>
+  <si>
+    <t>ResidentStatusOfPersonType</t>
+  </si>
+  <si>
+    <t>AggravatedAssaultHomicideCircum</t>
+  </si>
+  <si>
+    <t>AggravatedAssaultHomicideCircumstancesType</t>
+  </si>
+  <si>
+    <t>AdditionalJustificationHomicideCircumstancesType</t>
+  </si>
+  <si>
+    <t>AdditionalJustificationHomicideCi</t>
+  </si>
+  <si>
+    <t>TypeInjuryType</t>
+  </si>
+  <si>
+    <t>RelationshipsVictimToOffendersType</t>
+  </si>
+  <si>
+    <t>RelationshipsVictimToOffendersT</t>
+  </si>
+  <si>
+    <t>TypeOfArrestType</t>
+  </si>
+  <si>
+    <t>MultipleArresteeSegmentsIndicatorType</t>
+  </si>
+  <si>
+    <t>MultipleArresteeSegmentsIndicat</t>
+  </si>
+  <si>
+    <t>ArresteeWasArmedWithType</t>
+  </si>
+  <si>
+    <t>DispositionOfArresteeUnder18Type</t>
+  </si>
+  <si>
+    <t>DispositionOfArresteeUnder18Typ</t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1937,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="74">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1906,6 +2012,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1914,7 +2036,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="74">
+  <cellStyles count="90">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1951,6 +2073,14 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1987,6 +2117,14 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="73"/>
   </cellStyles>
@@ -2317,83 +2455,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>575</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>577</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>578</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
+        <v>578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>579</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
+        <v>579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>580</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>581</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>582</v>
+      </c>
+      <c r="B7" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>583</v>
+      </c>
+      <c r="B8" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>584</v>
+      </c>
+      <c r="B9" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>585</v>
+      </c>
+      <c r="B10" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>586</v>
+      </c>
+      <c r="B11" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>587</v>
+      </c>
+      <c r="B12" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>588</v>
+      </c>
+      <c r="B13" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>589</v>
+      </c>
+      <c r="B14" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>590</v>
+      </c>
+      <c r="B15" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>591</v>
+      </c>
+      <c r="B16" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>592</v>
+      </c>
+      <c r="B17" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>593</v>
+      </c>
+      <c r="B18" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>594</v>
+      </c>
+      <c r="B19" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>595</v>
+      </c>
+      <c r="B20" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>596</v>
+      </c>
+      <c r="B21" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>598</v>
+      </c>
+      <c r="B22" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>599</v>
+      </c>
+      <c r="B23" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>601</v>
+      </c>
+      <c r="B24" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>602</v>
+      </c>
+      <c r="B25" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>604</v>
+      </c>
+      <c r="B26" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>605</v>
+      </c>
+      <c r="B27" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>607</v>
+      </c>
+      <c r="B28" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>608</v>
+      </c>
+      <c r="B29" t="s">
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -2408,6 +2711,350 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2532,7 +3179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
@@ -3316,7 +3963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -3560,7 +4207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -3716,7 +4363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -3849,7 +4496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -4005,7 +4652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -4117,7 +4764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -4181,7 +4828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -4282,7 +4929,99 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -4351,104 +5090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -4515,7 +5157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -4737,7 +5379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -4846,7 +5488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -4968,7 +5610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
@@ -5288,7 +5930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -5353,7 +5995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -5417,7 +6059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -5591,7 +6233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -5645,6 +6287,103 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
@@ -6308,7 +7047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -6383,7 +7122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
@@ -6915,7 +7654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -6968,7 +7707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -7124,7 +7863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -7346,348 +8085,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>61</v>
-      </c>
-      <c r="C24" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>62</v>
-      </c>
-      <c r="C25" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>71</v>
-      </c>
-      <c r="C26" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>72</v>
-      </c>
-      <c r="C27" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>88</v>
-      </c>
-      <c r="C28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>99</v>
-      </c>
-      <c r="C29" t="s">
-        <v>281</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
made sure that every varchar had a precision and tested created the SQL
</commit_message>
<xml_diff>
--- a/r-load/NIBRSCodeTables.xlsx
+++ b/r-load/NIBRSCodeTables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="705"/>
@@ -2715,13 +2715,13 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3059,7 +3059,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3183,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3968,7 +3968,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4212,7 +4212,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4368,7 +4368,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4501,7 +4501,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4657,7 +4657,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4769,10 +4769,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -4832,8 +4835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4934,7 +4937,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5026,7 +5029,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5095,7 +5098,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5162,7 +5165,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5384,10 +5387,13 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
@@ -5493,7 +5499,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5615,7 +5621,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5934,7 +5940,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -6000,10 +6008,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -6064,10 +6075,13 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -6238,10 +6252,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -6291,10 +6308,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="176.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -6388,7 +6408,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A58"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7052,10 +7072,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -7126,8 +7149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7712,7 +7735,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7868,7 +7891,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>